<commit_message>
added switch buttons to website
</commit_message>
<xml_diff>
--- a/01_ProjectPlanning/05_ProductBacklock/ProductBacklock.xlsx
+++ b/01_ProjectPlanning/05_ProductBacklock/ProductBacklock.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Florian\3.Klasse\SYP\FoodScanner\01_ProjectPlanning\05_ProductBacklock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F739E056-D4AF-43E4-870C-AC00F5D900B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3607A23-09AF-4AC4-815D-C891113F4DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{AE588066-DD1E-46A9-8DEF-5F615E56FF65}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Tabelle1!$F$33:$F$50</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Tabelle1!$G$33:$G$50</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -224,11 +220,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -261,22 +256,31 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="25400" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent1">
+                    <a:alpha val="50000"/>
+                  </a:schemeClr>
                 </a:solidFill>
-                <a:prstDash val="sysDot"/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -376,8 +380,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
         <c:axId val="2004367151"/>
         <c:axId val="2004389199"/>
       </c:barChart>
@@ -394,14 +398,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -412,9 +410,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -441,12 +438,23 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -470,9 +478,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -508,11 +515,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -580,33 +590,46 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -615,38 +638,14 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -656,23 +655,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -680,71 +674,131 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:effectRef idx="0">
       <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -760,26 +814,47 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
+  </cs:downBar>
+  <cs:dropLine>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -787,35 +862,10 @@
       <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -827,14 +877,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -846,30 +895,35 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -879,16 +933,29 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -898,14 +965,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -917,14 +983,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -936,27 +1001,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -964,9 +1028,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -976,14 +1039,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -995,12 +1057,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1009,14 +1070,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1025,9 +1087,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1041,15 +1102,17 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1058,9 +1121,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1070,14 +1132,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1423,7 +1479,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>